<commit_message>
cập nhật theme  V1 071125
</commit_message>
<xml_diff>
--- a/data/curriculum_source_Topic1_G34.xlsx
+++ b/data/curriculum_source_Topic1_G34.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Downloads/IOSTEM-GenMap-Backup-2810/021125/GenMap/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290279C9-5B43-D747-91E7-5D00AF7B254A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43377537-AD4E-7648-85D3-3AB1ABC672E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="25100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -283,9 +283,6 @@
     <t>column_length:5; column_spacing:3; bar_position_offset:3; items_to_place:['switch','crystal','switch']; asset_theme:{'ground':'stone.stone02'}</t>
   </si>
   <si>
-    <t>Lệnh moveForward giúp nhân vật đi thẳng về phía trước 1 ô. Hãy kéo 3 khối lệnh moveForward vào khu vực lập trình để giúp nhân vật đi đến đích.</t>
-  </si>
-  <si>
     <t>The moveForward command makes the character walk one tile forward. Drag 3 moveForward blocks into the coding area to help the character reach the goal.</t>
   </si>
   <si>
@@ -1160,6 +1157,9 @@
   </si>
   <si>
     <t>G34</t>
+  </si>
+  <si>
+    <t>Lệnh moveForward giúp nhân vật đi thẳng về phía trước 1 ô. Hãy kéo 4 khối lệnh moveForward vào khu vực lập trình để giúp nhân vật đi đến đích.</t>
   </si>
 </sst>
 </file>
@@ -1436,7 +1436,7 @@
   <dimension ref="A1:AA55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1447,7 +1447,7 @@
     <col min="4" max="5" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="75.6640625" customWidth="1"/>
+    <col min="8" max="8" width="125.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="38" style="2" customWidth="1"/>
     <col min="11" max="11" width="19.5" bestFit="1" customWidth="1"/>
@@ -1521,7 +1521,7 @@
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>15</v>
@@ -1542,13 +1542,13 @@
         <v>25</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>87</v>
+        <v>379</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>50</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>39</v>
@@ -1580,7 +1580,7 @@
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>15</v>
@@ -1601,13 +1601,13 @@
         <v>52</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>53</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>39</v>
@@ -1639,7 +1639,7 @@
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>15</v>
@@ -1657,16 +1657,16 @@
         <v>3</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>56</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>57</v>
@@ -1698,7 +1698,7 @@
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>15</v>
@@ -1716,16 +1716,16 @@
         <v>4</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>39</v>
@@ -1737,7 +1737,7 @@
         <v>1</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>26</v>
@@ -1757,7 +1757,7 @@
     </row>
     <row r="6" spans="1:27" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>15</v>
@@ -1778,13 +1778,13 @@
         <v>43</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>44</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>39</v>
@@ -1796,7 +1796,7 @@
         <v>1</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>26</v>
@@ -1816,7 +1816,7 @@
     </row>
     <row r="7" spans="1:27" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>15</v>
@@ -1834,16 +1834,16 @@
         <v>6</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>57</v>
@@ -1855,7 +1855,7 @@
         <v>1</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>26</v>
@@ -1875,7 +1875,7 @@
     </row>
     <row r="8" spans="1:27" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>15</v>
@@ -1887,22 +1887,22 @@
         <v>16</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F8" s="1">
         <v>7</v>
       </c>
       <c r="G8" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>39</v>
@@ -1914,7 +1914,7 @@
         <v>1</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>28</v>
@@ -1934,7 +1934,7 @@
     </row>
     <row r="9" spans="1:27" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>15</v>
@@ -1946,7 +1946,7 @@
         <v>16</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F9" s="1">
         <v>8</v>
@@ -1955,13 +1955,13 @@
         <v>27</v>
       </c>
       <c r="H9" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>39</v>
@@ -1973,7 +1973,7 @@
         <v>1</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>28</v>
@@ -1993,7 +1993,7 @@
     </row>
     <row r="10" spans="1:27" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>15</v>
@@ -2005,22 +2005,22 @@
         <v>19</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F10" s="1">
         <v>9</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>22</v>
@@ -2032,7 +2032,7 @@
         <v>1</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>28</v>
@@ -2052,7 +2052,7 @@
     </row>
     <row r="11" spans="1:27" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>15</v>
@@ -2064,22 +2064,22 @@
         <v>19</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F11" s="1">
         <v>10</v>
       </c>
       <c r="G11" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>35</v>
@@ -2091,7 +2091,7 @@
         <v>1</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>28</v>
@@ -2111,7 +2111,7 @@
     </row>
     <row r="12" spans="1:27" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>15</v>
@@ -2123,7 +2123,7 @@
         <v>21</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F12" s="1">
         <v>11</v>
@@ -2132,13 +2132,13 @@
         <v>29</v>
       </c>
       <c r="H12" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>39</v>
@@ -2150,7 +2150,7 @@
         <v>1</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>28</v>
@@ -2170,7 +2170,7 @@
     </row>
     <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>15</v>
@@ -2182,22 +2182,22 @@
         <v>21</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F13" s="1">
         <v>12</v>
       </c>
       <c r="G13" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>39</v>
@@ -2209,7 +2209,7 @@
         <v>1</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>28</v>
@@ -2229,7 +2229,7 @@
     </row>
     <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>15</v>
@@ -2241,22 +2241,22 @@
         <v>16</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F14" s="1">
         <v>13</v>
       </c>
       <c r="G14" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>22</v>
@@ -2288,7 +2288,7 @@
     </row>
     <row r="15" spans="1:27" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>15</v>
@@ -2300,22 +2300,22 @@
         <v>16</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F15" s="1">
         <v>14</v>
       </c>
       <c r="G15" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>22</v>
@@ -2347,7 +2347,7 @@
     </row>
     <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>15</v>
@@ -2359,7 +2359,7 @@
         <v>16</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F16" s="1">
         <v>15</v>
@@ -2368,13 +2368,13 @@
         <v>64</v>
       </c>
       <c r="H16" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>154</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>65</v>
@@ -2406,7 +2406,7 @@
     </row>
     <row r="17" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>15</v>
@@ -2418,22 +2418,22 @@
         <v>19</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F17" s="1">
         <v>16</v>
       </c>
       <c r="G17" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>159</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>45</v>
@@ -2465,7 +2465,7 @@
     </row>
     <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>15</v>
@@ -2477,22 +2477,22 @@
         <v>19</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F18" s="1">
         <v>17</v>
       </c>
       <c r="G18" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>164</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>32</v>
@@ -2524,7 +2524,7 @@
     </row>
     <row r="19" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>15</v>
@@ -2536,22 +2536,22 @@
         <v>21</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F19" s="1">
         <v>18</v>
       </c>
       <c r="G19" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>22</v>
@@ -2563,7 +2563,7 @@
         <v>1</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O19" s="1" t="s">
         <v>28</v>
@@ -2572,7 +2572,7 @@
     </row>
     <row r="20" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>15</v>
@@ -2584,22 +2584,22 @@
         <v>21</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F20" s="1">
         <v>19</v>
       </c>
       <c r="G20" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="I20" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>175</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>45</v>
@@ -2611,7 +2611,7 @@
         <v>1</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="O20" s="1" t="s">
         <v>28</v>
@@ -2620,7 +2620,7 @@
     </row>
     <row r="21" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>15</v>
@@ -2632,22 +2632,22 @@
         <v>21</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F21" s="1">
         <v>20</v>
       </c>
       <c r="G21" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>179</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>83</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>32</v>
@@ -2659,7 +2659,7 @@
         <v>1</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O21" s="1" t="s">
         <v>28</v>
@@ -2668,7 +2668,7 @@
     </row>
     <row r="22" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>15</v>
@@ -2680,22 +2680,22 @@
         <v>16</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F22" s="1">
         <v>21</v>
       </c>
       <c r="G22" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="I22" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="J22" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>39</v>
@@ -2710,7 +2710,7 @@
         <v>70</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="P22" s="1" t="s">
         <v>18</v>
@@ -2718,7 +2718,7 @@
     </row>
     <row r="23" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>15</v>
@@ -2730,22 +2730,22 @@
         <v>16</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F23" s="1">
         <v>22</v>
       </c>
       <c r="G23" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="I23" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>192</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>57</v>
@@ -2760,7 +2760,7 @@
         <v>71</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="P23" s="1" t="s">
         <v>18</v>
@@ -2768,7 +2768,7 @@
     </row>
     <row r="24" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>15</v>
@@ -2780,22 +2780,22 @@
         <v>19</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F24" s="1">
         <v>23</v>
       </c>
       <c r="G24" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>195</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>72</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>22</v>
@@ -2807,10 +2807,10 @@
         <v>1</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="P24" s="1" t="s">
         <v>46</v>
@@ -2818,7 +2818,7 @@
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>15</v>
@@ -2830,22 +2830,22 @@
         <v>19</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F25" s="1">
         <v>24</v>
       </c>
       <c r="G25" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="I25" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="J25" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>73</v>
@@ -2857,10 +2857,10 @@
         <v>1</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="P25" s="1" t="s">
         <v>38</v>
@@ -2868,7 +2868,7 @@
     </row>
     <row r="26" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>15</v>
@@ -2880,22 +2880,22 @@
         <v>19</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F26" s="1">
         <v>25</v>
       </c>
       <c r="G26" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="I26" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="J26" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>208</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>45</v>
@@ -2907,10 +2907,10 @@
         <v>1</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="P26" s="1" t="s">
         <v>18</v>
@@ -2918,7 +2918,7 @@
     </row>
     <row r="27" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>15</v>
@@ -2930,22 +2930,22 @@
         <v>21</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F27" s="1">
         <v>26</v>
       </c>
       <c r="G27" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>212</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>74</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>39</v>
@@ -2957,10 +2957,10 @@
         <v>1</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="P27" s="1" t="s">
         <v>18</v>
@@ -2968,7 +2968,7 @@
     </row>
     <row r="28" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>15</v>
@@ -2980,22 +2980,22 @@
         <v>21</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F28" s="1">
         <v>27</v>
       </c>
       <c r="G28" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="I28" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="J28" s="1" t="s">
         <v>218</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>219</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>22</v>
@@ -3007,10 +3007,10 @@
         <v>1</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="P28" s="1" t="s">
         <v>18</v>
@@ -3018,7 +3018,7 @@
     </row>
     <row r="29" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>15</v>
@@ -3030,22 +3030,22 @@
         <v>21</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F29" s="1">
         <v>28</v>
       </c>
       <c r="G29" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="I29" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="I29" s="1" t="s">
+      <c r="J29" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>225</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>73</v>
@@ -3057,10 +3057,10 @@
         <v>1</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="P29" s="1" t="s">
         <v>46</v>
@@ -3068,7 +3068,7 @@
     </row>
     <row r="30" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>15</v>
@@ -3080,7 +3080,7 @@
         <v>16</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F30" s="1">
         <v>29</v>
@@ -3089,13 +3089,13 @@
         <v>30</v>
       </c>
       <c r="H30" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="I30" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="I30" s="1" t="s">
+      <c r="J30" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>230</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>17</v>
@@ -3118,7 +3118,7 @@
     </row>
     <row r="31" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>15</v>
@@ -3130,22 +3130,22 @@
         <v>16</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F31" s="1">
         <v>30</v>
       </c>
       <c r="G31" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="I31" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="I31" s="1" t="s">
+      <c r="J31" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>57</v>
@@ -3168,7 +3168,7 @@
     </row>
     <row r="32" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>15</v>
@@ -3180,22 +3180,22 @@
         <v>19</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F32" s="1">
         <v>31</v>
       </c>
       <c r="G32" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="H32" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="I32" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="I32" s="1" t="s">
+      <c r="J32" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>240</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>45</v>
@@ -3218,7 +3218,7 @@
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>15</v>
@@ -3230,22 +3230,22 @@
         <v>19</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F33" s="1">
         <v>32</v>
       </c>
       <c r="G33" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="I33" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="I33" s="1" t="s">
+      <c r="J33" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>245</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>78</v>
@@ -3268,7 +3268,7 @@
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>15</v>
@@ -3280,34 +3280,34 @@
         <v>19</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F34" s="1">
         <v>33</v>
       </c>
       <c r="G34" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="I34" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="I34" s="1" t="s">
+      <c r="J34" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="J34" s="1" t="s">
+      <c r="K34" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="K34" s="1" t="s">
+      <c r="L34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M34" s="1">
+        <v>1</v>
+      </c>
+      <c r="N34" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="L34" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M34" s="1">
-        <v>1</v>
-      </c>
-      <c r="N34" s="1" t="s">
-        <v>252</v>
       </c>
       <c r="O34" s="1" t="s">
         <v>41</v>
@@ -3318,7 +3318,7 @@
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>15</v>
@@ -3330,22 +3330,22 @@
         <v>21</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F35" s="1">
         <v>34</v>
       </c>
       <c r="G35" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="H35" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="I35" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="I35" s="1" t="s">
+      <c r="J35" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>257</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>17</v>
@@ -3357,7 +3357,7 @@
         <v>1</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="O35" s="1" t="s">
         <v>41</v>
@@ -3368,7 +3368,7 @@
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>15</v>
@@ -3380,22 +3380,22 @@
         <v>21</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F36" s="1">
         <v>35</v>
       </c>
       <c r="G36" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="H36" s="1" t="s">
         <v>260</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>261</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>80</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>45</v>
@@ -3407,7 +3407,7 @@
         <v>1</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="O36" s="1" t="s">
         <v>41</v>
@@ -3418,7 +3418,7 @@
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>15</v>
@@ -3430,22 +3430,22 @@
         <v>21</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F37" s="1">
         <v>36</v>
       </c>
       <c r="G37" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="H37" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="I37" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="I37" s="1" t="s">
+      <c r="J37" s="1" t="s">
         <v>267</v>
-      </c>
-      <c r="J37" s="1" t="s">
-        <v>268</v>
       </c>
       <c r="K37" s="1" t="s">
         <v>78</v>
@@ -3457,7 +3457,7 @@
         <v>1</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="O37" s="1" t="s">
         <v>41</v>
@@ -3468,7 +3468,7 @@
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>15</v>
@@ -3480,22 +3480,22 @@
         <v>19</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F38" s="1">
         <v>37</v>
       </c>
       <c r="G38" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="H38" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="I38" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="I38" s="1" t="s">
+      <c r="J38" s="1" t="s">
         <v>273</v>
-      </c>
-      <c r="J38" s="1" t="s">
-        <v>274</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>45</v>
@@ -3513,12 +3513,12 @@
         <v>41</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>15</v>
@@ -3530,45 +3530,45 @@
         <v>19</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F39" s="1">
         <v>38</v>
       </c>
       <c r="G39" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="H39" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="I39" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="I39" s="1" t="s">
+      <c r="J39" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="J39" s="1" t="s">
+      <c r="K39" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M39" s="1">
+        <v>1</v>
+      </c>
+      <c r="N39" s="1" t="s">
         <v>280</v>
-      </c>
-      <c r="K39" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="L39" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M39" s="1">
-        <v>1</v>
-      </c>
-      <c r="N39" s="1" t="s">
-        <v>281</v>
       </c>
       <c r="O39" s="1" t="s">
         <v>41</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>15</v>
@@ -3580,22 +3580,22 @@
         <v>19</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F40" s="1">
         <v>39</v>
       </c>
       <c r="G40" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="H40" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="I40" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="I40" s="1" t="s">
+      <c r="J40" s="1" t="s">
         <v>285</v>
-      </c>
-      <c r="J40" s="1" t="s">
-        <v>286</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>78</v>
@@ -3607,7 +3607,7 @@
         <v>1</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="O40" s="1" t="s">
         <v>41</v>
@@ -3618,7 +3618,7 @@
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>15</v>
@@ -3636,16 +3636,16 @@
         <v>40</v>
       </c>
       <c r="G41" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="H41" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="I41" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="I41" s="1" t="s">
+      <c r="J41" s="1" t="s">
         <v>290</v>
-      </c>
-      <c r="J41" s="1" t="s">
-        <v>291</v>
       </c>
       <c r="K41" s="1" t="s">
         <v>42</v>
@@ -3657,18 +3657,18 @@
         <v>1</v>
       </c>
       <c r="N41" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="O41" s="1" t="s">
         <v>41</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>15</v>
@@ -3680,22 +3680,22 @@
         <v>21</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F42" s="1">
         <v>41</v>
       </c>
       <c r="G42" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="H42" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="I42" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="I42" s="1" t="s">
+      <c r="J42" s="1" t="s">
         <v>296</v>
-      </c>
-      <c r="J42" s="1" t="s">
-        <v>297</v>
       </c>
       <c r="K42" s="1" t="s">
         <v>45</v>
@@ -3707,18 +3707,18 @@
         <v>1</v>
       </c>
       <c r="N42" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="O42" s="1" t="s">
         <v>41</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>15</v>
@@ -3730,22 +3730,22 @@
         <v>21</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F43" s="1">
         <v>42</v>
       </c>
       <c r="G43" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="H43" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="I43" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="I43" s="1" t="s">
+      <c r="J43" s="1" t="s">
         <v>302</v>
-      </c>
-      <c r="J43" s="1" t="s">
-        <v>303</v>
       </c>
       <c r="K43" s="1" t="s">
         <v>78</v>
@@ -3757,7 +3757,7 @@
         <v>1</v>
       </c>
       <c r="N43" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="O43" s="1" t="s">
         <v>41</v>
@@ -3768,7 +3768,7 @@
     </row>
     <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>15</v>
@@ -3780,34 +3780,34 @@
         <v>21</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F44" s="1">
         <v>43</v>
       </c>
       <c r="G44" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="H44" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="I44" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="I44" s="1" t="s">
+      <c r="J44" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="J44" s="1" t="s">
+      <c r="K44" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M44" s="1">
+        <v>1</v>
+      </c>
+      <c r="N44" s="1" t="s">
         <v>309</v>
-      </c>
-      <c r="K44" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="L44" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M44" s="1">
-        <v>1</v>
-      </c>
-      <c r="N44" s="1" t="s">
-        <v>310</v>
       </c>
       <c r="O44" s="1" t="s">
         <v>41</v>
@@ -3818,7 +3818,7 @@
     </row>
     <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>15</v>
@@ -3830,22 +3830,22 @@
         <v>21</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F45" s="1">
         <v>44</v>
       </c>
       <c r="G45" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="H45" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="H45" s="1" t="s">
+      <c r="I45" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="I45" s="1" t="s">
+      <c r="J45" s="1" t="s">
         <v>314</v>
-      </c>
-      <c r="J45" s="1" t="s">
-        <v>315</v>
       </c>
       <c r="K45" s="1" t="s">
         <v>68</v>
@@ -3857,18 +3857,18 @@
         <v>1</v>
       </c>
       <c r="N45" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="O45" s="1" t="s">
         <v>41</v>
       </c>
       <c r="P45" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>15</v>
@@ -3880,22 +3880,22 @@
         <v>21</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F46" s="1">
         <v>45</v>
       </c>
       <c r="G46" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="H46" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="I46" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="I46" s="1" t="s">
+      <c r="J46" s="1" t="s">
         <v>320</v>
-      </c>
-      <c r="J46" s="1" t="s">
-        <v>321</v>
       </c>
       <c r="K46" s="1" t="s">
         <v>65</v>
@@ -3907,18 +3907,18 @@
         <v>1</v>
       </c>
       <c r="N46" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="O46" s="1" t="s">
         <v>41</v>
       </c>
       <c r="P46" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>15</v>
@@ -3936,16 +3936,16 @@
         <v>46</v>
       </c>
       <c r="G47" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="H47" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="I47" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="I47" s="1" t="s">
+      <c r="J47" s="1" t="s">
         <v>325</v>
-      </c>
-      <c r="J47" s="1" t="s">
-        <v>326</v>
       </c>
       <c r="K47" s="1" t="s">
         <v>73</v>
@@ -3957,18 +3957,18 @@
         <v>1</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="O47" s="1" t="s">
         <v>41</v>
       </c>
       <c r="P47" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="48" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>15</v>
@@ -3986,16 +3986,16 @@
         <v>47</v>
       </c>
       <c r="G48" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="H48" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="I48" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="I48" s="1" t="s">
+      <c r="J48" s="1" t="s">
         <v>331</v>
-      </c>
-      <c r="J48" s="1" t="s">
-        <v>332</v>
       </c>
       <c r="K48" s="1" t="s">
         <v>78</v>
@@ -4013,12 +4013,12 @@
         <v>41</v>
       </c>
       <c r="P48" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="49" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>15</v>
@@ -4030,34 +4030,34 @@
         <v>19</v>
       </c>
       <c r="E49" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="F49" s="1">
+        <v>48</v>
+      </c>
+      <c r="G49" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="F49" s="1">
-        <v>48</v>
-      </c>
-      <c r="G49" s="1" t="s">
+      <c r="H49" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="H49" s="1" t="s">
+      <c r="I49" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="I49" s="1" t="s">
+      <c r="J49" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="J49" s="1" t="s">
+      <c r="K49" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="K49" s="1" t="s">
+      <c r="L49" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M49" s="1">
+        <v>1</v>
+      </c>
+      <c r="N49" s="1" t="s">
         <v>339</v>
-      </c>
-      <c r="L49" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M49" s="1">
-        <v>1</v>
-      </c>
-      <c r="N49" s="1" t="s">
-        <v>340</v>
       </c>
       <c r="O49" s="1" t="s">
         <v>41</v>
@@ -4068,7 +4068,7 @@
     </row>
     <row r="50" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>15</v>
@@ -4080,22 +4080,22 @@
         <v>21</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F50" s="1">
         <v>49</v>
       </c>
       <c r="G50" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="H50" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="H50" s="1" t="s">
+      <c r="I50" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="I50" s="1" t="s">
+      <c r="J50" s="1" t="s">
         <v>344</v>
-      </c>
-      <c r="J50" s="1" t="s">
-        <v>345</v>
       </c>
       <c r="K50" s="1" t="s">
         <v>42</v>
@@ -4107,7 +4107,7 @@
         <v>1</v>
       </c>
       <c r="N50" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="O50" s="1" t="s">
         <v>41</v>
@@ -4118,7 +4118,7 @@
     </row>
     <row r="51" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>15</v>
@@ -4130,34 +4130,34 @@
         <v>19</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F51" s="1">
         <v>50</v>
       </c>
       <c r="G51" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="H51" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="H51" s="1" t="s">
+      <c r="I51" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="I51" s="1" t="s">
+      <c r="J51" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="J51" s="1" t="s">
+      <c r="K51" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="K51" s="1" t="s">
+      <c r="L51" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M51" s="1">
+        <v>1</v>
+      </c>
+      <c r="N51" s="1" t="s">
         <v>352</v>
-      </c>
-      <c r="L51" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M51" s="1">
-        <v>1</v>
-      </c>
-      <c r="N51" s="1" t="s">
-        <v>353</v>
       </c>
       <c r="O51" s="1" t="s">
         <v>41</v>
@@ -4168,7 +4168,7 @@
     </row>
     <row r="52" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>15</v>
@@ -4180,34 +4180,34 @@
         <v>19</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F52" s="1">
         <v>51</v>
       </c>
       <c r="G52" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="H52" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="H52" s="1" t="s">
+      <c r="I52" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="I52" s="1" t="s">
+      <c r="J52" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="J52" s="1" t="s">
+      <c r="K52" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="K52" s="1" t="s">
+      <c r="L52" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M52" s="1">
+        <v>1</v>
+      </c>
+      <c r="N52" s="1" t="s">
         <v>359</v>
-      </c>
-      <c r="L52" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M52" s="1">
-        <v>1</v>
-      </c>
-      <c r="N52" s="1" t="s">
-        <v>360</v>
       </c>
       <c r="O52" s="1" t="s">
         <v>41</v>
@@ -4218,7 +4218,7 @@
     </row>
     <row r="53" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>15</v>
@@ -4230,22 +4230,22 @@
         <v>21</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F53" s="1">
         <v>52</v>
       </c>
       <c r="G53" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="H53" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="H53" s="1" t="s">
+      <c r="I53" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="I53" s="1" t="s">
+      <c r="J53" s="1" t="s">
         <v>364</v>
-      </c>
-      <c r="J53" s="1" t="s">
-        <v>365</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>37</v>
@@ -4257,7 +4257,7 @@
         <v>1</v>
       </c>
       <c r="N53" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="O53" s="1" t="s">
         <v>41</v>
@@ -4268,7 +4268,7 @@
     </row>
     <row r="54" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>15</v>
@@ -4280,22 +4280,22 @@
         <v>19</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F54" s="1">
         <v>53</v>
       </c>
       <c r="G54" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="H54" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="H54" s="1" t="s">
+      <c r="I54" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="I54" s="1" t="s">
+      <c r="J54" s="1" t="s">
         <v>370</v>
-      </c>
-      <c r="J54" s="1" t="s">
-        <v>371</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>20</v>
@@ -4307,18 +4307,18 @@
         <v>1</v>
       </c>
       <c r="N54" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="O54" s="1" t="s">
         <v>41</v>
       </c>
       <c r="P54" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="55" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>15</v>
@@ -4330,22 +4330,22 @@
         <v>19</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F55" s="1">
         <v>54</v>
       </c>
       <c r="G55" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="H55" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="H55" s="1" t="s">
+      <c r="I55" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="I55" s="1" t="s">
+      <c r="J55" s="1" t="s">
         <v>376</v>
-      </c>
-      <c r="J55" s="1" t="s">
-        <v>377</v>
       </c>
       <c r="K55" s="1" t="s">
         <v>36</v>
@@ -4357,13 +4357,13 @@
         <v>1</v>
       </c>
       <c r="N55" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="O55" s="1" t="s">
         <v>41</v>
       </c>
       <c r="P55" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>

</xml_diff>